<commit_message>
scoring older adult output
</commit_message>
<xml_diff>
--- a/CVOE/5 Manuscript/Output/Older MCI Output 10_14.xlsx
+++ b/CVOE/5 Manuscript/Output/Older MCI Output 10_14.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm\Documents\GitHub\Spring-2019-Projects\CVOE\5 Manuscript\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm\OneDrive\Documents\GitHub\Spring-2019-Projects\CVOE\5 Manuscript\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077A03C4-E21E-493A-A9FC-C5F0D7546B68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{077A03C4-E21E-493A-A9FC-C5F0D7546B68}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{AAB180F1-A786-4A75-9657-9EA7E2721A71}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" activeTab="1" xr2:uid="{E0C5538E-1FAD-433E-AC4C-D2EEA76FE06A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E0C5538E-1FAD-433E-AC4C-D2EEA76FE06A}"/>
   </bookViews>
   <sheets>
     <sheet name="Errors" sheetId="1" r:id="rId1"/>
@@ -513,15 +513,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE5C1B3-1D15-409E-BB0E-BB269A9102CD}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +559,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2001</v>
       </c>
@@ -567,37 +567,37 @@
         <v>6.25E-2</v>
       </c>
       <c r="C2">
-        <v>0.42528735632183901</v>
+        <v>0.435294117647059</v>
       </c>
       <c r="D2">
-        <v>0.24389367816092</v>
+        <v>0.248897058823529</v>
       </c>
       <c r="E2">
-        <v>0.55102040816326503</v>
+        <v>0.565217391304348</v>
       </c>
       <c r="F2">
         <v>0.41176470588235298</v>
       </c>
       <c r="G2">
-        <v>0.51666666666666705</v>
+        <v>0.50847457627118597</v>
       </c>
       <c r="H2">
         <v>0.43859649122806998</v>
       </c>
       <c r="I2">
-        <v>0.167871027721433</v>
+        <v>0.16286764705882401</v>
       </c>
       <c r="J2">
-        <v>0.19470281306715101</v>
+        <v>0.18969943240454101</v>
       </c>
       <c r="K2">
-        <v>0.139255702280912</v>
+        <v>0.153452685421995</v>
       </c>
       <c r="L2">
-        <v>7.8070175438596401E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6.9878085043116198E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2002</v>
       </c>
@@ -611,7 +611,7 @@
         <v>0.157510964912281</v>
       </c>
       <c r="E3">
-        <v>0.25490196078431399</v>
+        <v>0.26086956521739102</v>
       </c>
       <c r="F3">
         <v>0.145454545454546</v>
@@ -629,24 +629,24 @@
         <v>0.23904075922564999</v>
       </c>
       <c r="K3">
-        <v>0.109447415329768</v>
+        <v>0.115415019762846</v>
       </c>
       <c r="L3">
         <v>-3.5895986433013102E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2003</v>
       </c>
       <c r="B4">
-        <v>4.5977011494252901E-2</v>
+        <v>4.7058823529411799E-2</v>
       </c>
       <c r="C4">
-        <v>8.6956521739130502E-2</v>
+        <v>8.8888888888888906E-2</v>
       </c>
       <c r="D4">
-        <v>6.6466766616691694E-2</v>
+        <v>6.7973856209150404E-2</v>
       </c>
       <c r="E4">
         <v>0.28813559322033899</v>
@@ -661,10 +661,10 @@
         <v>0.29310344827586199</v>
       </c>
       <c r="I4">
-        <v>0.133533233383308</v>
+        <v>0.13202614379085001</v>
       </c>
       <c r="J4">
-        <v>0.22663668165917</v>
+        <v>0.22512959206671199</v>
       </c>
       <c r="K4">
         <v>8.8135593220338995E-2</v>
@@ -673,7 +673,7 @@
         <v>-3.0808366308648999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2004</v>
       </c>
@@ -681,13 +681,13 @@
         <v>2.1052631578947299E-2</v>
       </c>
       <c r="C5">
-        <v>1.04166666666666E-2</v>
+        <v>1.05263157894737E-2</v>
       </c>
       <c r="D5">
-        <v>1.5734649122807001E-2</v>
+        <v>1.5789473684210499E-2</v>
       </c>
       <c r="E5">
-        <v>0.13559322033898299</v>
+        <v>0.12280701754386</v>
       </c>
       <c r="F5">
         <v>8.4745762711864403E-2</v>
@@ -699,19 +699,19 @@
         <v>3.5087719298245598E-2</v>
       </c>
       <c r="I5">
-        <v>6.9011113589057399E-2</v>
+        <v>6.8956289027653897E-2</v>
       </c>
       <c r="J5">
-        <v>1.9353070175438601E-2</v>
+        <v>1.9298245614035099E-2</v>
       </c>
       <c r="K5">
-        <v>5.0847457627118599E-2</v>
+        <v>3.8061254831995302E-2</v>
       </c>
       <c r="L5">
         <v>6.4912280701754393E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2006</v>
       </c>
@@ -749,7 +749,7 @@
         <v>-5.1724137931034503E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2007</v>
       </c>
@@ -763,7 +763,7 @@
         <v>1.0639501980758401E-2</v>
       </c>
       <c r="E7">
-        <v>5.2631578947368501E-2</v>
+        <v>5.4545454545454598E-2</v>
       </c>
       <c r="F7">
         <v>3.5714285714285698E-2</v>
@@ -781,13 +781,13 @@
         <v>-1.0639501980758401E-2</v>
       </c>
       <c r="K7">
-        <v>1.69172932330828E-2</v>
+        <v>1.88311688311689E-2</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2009</v>
       </c>
@@ -825,7 +825,7 @@
         <v>7.6502732240437105E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2010</v>
       </c>
@@ -863,7 +863,7 @@
         <v>-1.3566986998304199E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2011</v>
       </c>
@@ -877,13 +877,13 @@
         <v>9.4414893617021295E-2</v>
       </c>
       <c r="E10">
-        <v>0.24561403508771901</v>
+        <v>0.25</v>
       </c>
       <c r="F10">
         <v>0.214285714285714</v>
       </c>
       <c r="G10">
-        <v>8.3333333333333398E-2</v>
+        <v>8.4745762711864403E-2</v>
       </c>
       <c r="H10">
         <v>1.6949152542372801E-2</v>
@@ -895,13 +895,13 @@
         <v>-7.7465741074648403E-2</v>
       </c>
       <c r="K10">
-        <v>3.1328320802004997E-2</v>
+        <v>3.5714285714285698E-2</v>
       </c>
       <c r="L10">
-        <v>6.6384180790960506E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6.7796610169491595E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2012</v>
       </c>
@@ -939,7 +939,7 @@
         <v>-1.75048624617949E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -977,7 +977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>3.3064740205612703E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2017</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>0.101694915254237</v>
       </c>
       <c r="F14">
-        <v>1.6666666666666701E-2</v>
+        <v>1.6949152542372801E-2</v>
       </c>
       <c r="G14">
         <v>1.63934426229508E-2</v>
@@ -1041,19 +1041,19 @@
         <v>3.4482758620689599E-2</v>
       </c>
       <c r="I14">
-        <v>-9.3749999999999702E-3</v>
+        <v>-9.0925141242938507E-3</v>
       </c>
       <c r="J14">
         <v>8.4410919540229296E-3</v>
       </c>
       <c r="K14">
-        <v>8.5028248587570507E-2</v>
+        <v>8.4745762711864403E-2</v>
       </c>
       <c r="L14">
         <v>-1.8089315997738799E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2019</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>-6.7834934991520797E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2020</v>
       </c>
@@ -1129,336 +1129,678 @@
         <v>-1.6110797060486098E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
+        <v>2021</v>
+      </c>
+      <c r="B17">
+        <v>1.04166666666666E-2</v>
+      </c>
+      <c r="C17">
+        <v>0.28125</v>
+      </c>
+      <c r="D17">
+        <v>0.14583333333333301</v>
+      </c>
+      <c r="E17">
+        <v>0.186440677966102</v>
+      </c>
+      <c r="F17">
+        <v>0.16393442622950799</v>
+      </c>
+      <c r="G17">
+        <v>0.19672131147541</v>
+      </c>
+      <c r="H17">
+        <v>0.13559322033898299</v>
+      </c>
+      <c r="I17">
+        <v>1.81010928961748E-2</v>
+      </c>
+      <c r="J17">
+        <v>-1.0240112994350299E-2</v>
+      </c>
+      <c r="K17">
+        <v>2.2506251736593499E-2</v>
+      </c>
+      <c r="L17">
+        <v>6.1128091136426803E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2022</v>
+      </c>
+      <c r="B18">
+        <v>1.04166666666666E-2</v>
+      </c>
+      <c r="C18">
+        <v>1.05263157894737E-2</v>
+      </c>
+      <c r="D18">
+        <v>1.0471491228070199E-2</v>
+      </c>
+      <c r="E18">
+        <v>5.1724137931034503E-2</v>
+      </c>
+      <c r="F18">
+        <v>1.6666666666666701E-2</v>
+      </c>
+      <c r="G18">
+        <v>4.91803278688525E-2</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>6.1951754385965504E-3</v>
+      </c>
+      <c r="J18">
+        <v>-1.0471491228070199E-2</v>
+      </c>
+      <c r="K18">
+        <v>3.5057471264367798E-2</v>
+      </c>
+      <c r="L18">
+        <v>4.91803278688525E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>2023</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <v>2.0833333333333402E-2</v>
       </c>
-      <c r="C17">
+      <c r="C19">
         <v>2.0833333333333402E-2</v>
       </c>
-      <c r="D17">
+      <c r="D19">
         <v>2.0833333333333402E-2</v>
       </c>
-      <c r="E17">
+      <c r="E19">
+        <v>0.114754098360656</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
         <v>1.6949152542372801E-2</v>
       </c>
-      <c r="F17">
+      <c r="H19">
         <v>0</v>
       </c>
-      <c r="G17">
+      <c r="I19">
+        <v>-2.0833333333333402E-2</v>
+      </c>
+      <c r="J19">
+        <v>-2.0833333333333402E-2</v>
+      </c>
+      <c r="K19">
         <v>0.114754098360656</v>
       </c>
-      <c r="H17">
+      <c r="L19">
+        <v>1.6949152542372801E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2024</v>
+      </c>
+      <c r="B20">
+        <v>7.2916666666666602E-2</v>
+      </c>
+      <c r="C20">
+        <v>0.13684210526315799</v>
+      </c>
+      <c r="D20">
+        <v>0.104879385964912</v>
+      </c>
+      <c r="E20">
+        <v>0.10344827586206901</v>
+      </c>
+      <c r="F20">
+        <v>3.3333333333333298E-2</v>
+      </c>
+      <c r="G20">
+        <v>0.2</v>
+      </c>
+      <c r="H20">
+        <v>0.20689655172413801</v>
+      </c>
+      <c r="I20">
+        <v>-7.1546052631578899E-2</v>
+      </c>
+      <c r="J20">
+        <v>0.10201716575922599</v>
+      </c>
+      <c r="K20">
+        <v>7.0114942528735597E-2</v>
+      </c>
+      <c r="L20">
+        <v>-6.8965517241379396E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2025</v>
+      </c>
+      <c r="B21">
+        <v>1.04166666666666E-2</v>
+      </c>
+      <c r="C21">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D21">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="E21">
+        <v>8.77192982456141E-2</v>
+      </c>
+      <c r="F21">
+        <v>3.3333333333333298E-2</v>
+      </c>
+      <c r="G21">
         <v>0</v>
       </c>
-      <c r="I17">
+      <c r="H21">
+        <v>1.75438596491229E-2</v>
+      </c>
+      <c r="I21">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="J21">
+        <v>-3.2894736842104498E-3</v>
+      </c>
+      <c r="K21">
+        <v>5.4385964912280801E-2</v>
+      </c>
+      <c r="L21">
+        <v>-1.75438596491229E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2026</v>
+      </c>
+      <c r="B22">
+        <v>4.1666666666666602E-2</v>
+      </c>
+      <c r="C22">
+        <v>2.0833333333333402E-2</v>
+      </c>
+      <c r="D22">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E22">
+        <v>5.0847457627118599E-2</v>
+      </c>
+      <c r="F22">
+        <v>3.4482758620689599E-2</v>
+      </c>
+      <c r="G22">
+        <v>4.91803278688525E-2</v>
+      </c>
+      <c r="H22">
+        <v>1.72413793103449E-2</v>
+      </c>
+      <c r="I22">
+        <v>3.23275862068961E-3</v>
+      </c>
+      <c r="J22">
+        <v>-1.40086206896551E-2</v>
+      </c>
+      <c r="K22">
+        <v>1.6364699006429E-2</v>
+      </c>
+      <c r="L22">
+        <v>3.19389485585077E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2027</v>
+      </c>
+      <c r="B23">
+        <v>2.1052631578947299E-2</v>
+      </c>
+      <c r="C23">
+        <v>3.1914893617021302E-2</v>
+      </c>
+      <c r="D23">
+        <v>2.6483762597984298E-2</v>
+      </c>
+      <c r="E23">
+        <v>1.75438596491229E-2</v>
+      </c>
+      <c r="F23">
+        <v>3.5087719298245598E-2</v>
+      </c>
+      <c r="G23">
+        <v>6.6666666666666693E-2</v>
+      </c>
+      <c r="H23">
+        <v>1.72413793103449E-2</v>
+      </c>
+      <c r="I23">
+        <v>8.6039567002613206E-3</v>
+      </c>
+      <c r="J23">
+        <v>-9.2423832876394295E-3</v>
+      </c>
+      <c r="K23">
+        <v>-1.7543859649122799E-2</v>
+      </c>
+      <c r="L23">
+        <v>4.9425287356321797E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2028</v>
+      </c>
+      <c r="B24">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C24">
+        <v>1.04166666666666E-2</v>
+      </c>
+      <c r="D24">
+        <v>3.6458333333333301E-2</v>
+      </c>
+      <c r="E24">
+        <v>8.1967213114754106E-2</v>
+      </c>
+      <c r="F24">
+        <v>1.72413793103449E-2</v>
+      </c>
+      <c r="G24">
+        <v>5.0847457627118599E-2</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>-1.9216954022988501E-2</v>
+      </c>
+      <c r="J24">
+        <v>-3.6458333333333301E-2</v>
+      </c>
+      <c r="K24">
+        <v>6.4725833804409202E-2</v>
+      </c>
+      <c r="L24">
+        <v>5.0847457627118599E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2029</v>
+      </c>
+      <c r="B25">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C25">
+        <v>8.3333333333333398E-2</v>
+      </c>
+      <c r="D25">
+        <v>5.7291666666666699E-2</v>
+      </c>
+      <c r="E25">
+        <v>8.4745762711864403E-2</v>
+      </c>
+      <c r="F25">
+        <v>8.3333333333333398E-2</v>
+      </c>
+      <c r="G25">
+        <v>6.5573770491803199E-2</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>2.6041666666666699E-2</v>
+      </c>
+      <c r="J25">
+        <v>-5.7291666666666699E-2</v>
+      </c>
+      <c r="K25">
+        <v>1.4124293785310301E-3</v>
+      </c>
+      <c r="L25">
+        <v>6.5573770491803199E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2031</v>
+      </c>
+      <c r="B26">
+        <v>2.0833333333333402E-2</v>
+      </c>
+      <c r="C26">
+        <v>2.0833333333333402E-2</v>
+      </c>
+      <c r="D26">
+        <v>2.0833333333333402E-2</v>
+      </c>
+      <c r="E26">
+        <v>3.3898305084745797E-2</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>4.91803278688525E-2</v>
+      </c>
+      <c r="H26">
+        <v>1.6949152542372801E-2</v>
+      </c>
+      <c r="I26">
         <v>-2.0833333333333402E-2</v>
       </c>
-      <c r="J17">
-        <v>-2.0833333333333402E-2</v>
-      </c>
-      <c r="K17">
-        <v>1.6949152542372801E-2</v>
-      </c>
-      <c r="L17">
-        <v>0.114754098360656</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="J26">
+        <v>-3.8841807909605298E-3</v>
+      </c>
+      <c r="K26">
+        <v>3.3898305084745797E-2</v>
+      </c>
+      <c r="L26">
+        <v>3.2231175326479698E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B19">
-        <f>AVERAGE(B2:B17)</f>
-        <v>3.4892278261618302E-2</v>
-      </c>
-      <c r="C19">
-        <f t="shared" ref="C19:L19" si="0">AVERAGE(C2:C17)</f>
-        <v>9.6907838730061036E-2</v>
-      </c>
-      <c r="D19">
+      <c r="B29">
+        <f>AVERAGE(B2:B26)</f>
+        <v>3.363310249866662E-2</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:L29" si="0">AVERAGE(C2:C26)</f>
+        <v>8.7590967144603293E-2</v>
+      </c>
+      <c r="D29">
         <f t="shared" si="0"/>
-        <v>6.5900058495839769E-2</v>
-      </c>
-      <c r="E19">
+        <v>6.061203482163495E-2</v>
+      </c>
+      <c r="E29">
         <f t="shared" si="0"/>
-        <v>0.21205550185868433</v>
-      </c>
-      <c r="F19">
+        <v>0.16810824756156248</v>
+      </c>
+      <c r="F29">
         <f t="shared" si="0"/>
-        <v>0.15241669769457239</v>
-      </c>
-      <c r="G19">
+        <v>0.11425450396457276</v>
+      </c>
+      <c r="G29">
         <f t="shared" si="0"/>
-        <v>0.19436475409836076</v>
-      </c>
-      <c r="H19">
+        <v>0.14930406594424378</v>
+      </c>
+      <c r="H29">
         <f t="shared" si="0"/>
-        <v>0.17916448778287039</v>
-      </c>
-      <c r="I19">
+        <v>0.13112389389604931</v>
+      </c>
+      <c r="I29">
         <f t="shared" si="0"/>
-        <v>8.6516639198732648E-2</v>
-      </c>
-      <c r="J19">
+        <v>5.3642469142937833E-2</v>
+      </c>
+      <c r="J29">
         <f t="shared" si="0"/>
-        <v>0.11326442928703073</v>
-      </c>
-      <c r="K19">
+        <v>7.0511859074414429E-2</v>
+      </c>
+      <c r="K29">
         <f t="shared" si="0"/>
-        <v>5.9638804164111964E-2</v>
-      </c>
-      <c r="L19">
+        <v>5.3853743596989717E-2</v>
+      </c>
+      <c r="L29">
         <f t="shared" si="0"/>
-        <v>1.5200266315490277E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+        <v>1.8180172048194464E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B20">
-        <f>STDEV(B2:B17)</f>
-        <v>3.1625997844064294E-2</v>
-      </c>
-      <c r="C20">
-        <f t="shared" ref="C20:L20" si="1">STDEV(C2:C17)</f>
-        <v>0.12286998252178144</v>
-      </c>
-      <c r="D20">
+      <c r="B30">
+        <f>STDEV(B2:B26)</f>
+        <v>2.8462055809265429E-2</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:L30" si="1">STDEV(C2:C26)</f>
+        <v>0.11212290566961883</v>
+      </c>
+      <c r="D30">
         <f t="shared" si="1"/>
-        <v>7.0200153509582211E-2</v>
-      </c>
-      <c r="E20">
+        <v>6.2504916885516681E-2</v>
+      </c>
+      <c r="E30">
         <f t="shared" si="1"/>
-        <v>0.18314273538599266</v>
-      </c>
-      <c r="F20">
+        <v>0.16082414606833834</v>
+      </c>
+      <c r="F30">
         <f t="shared" si="1"/>
-        <v>0.13555214513353681</v>
-      </c>
-      <c r="G20">
+        <v>0.12247499319888792</v>
+      </c>
+      <c r="G30">
         <f t="shared" si="1"/>
-        <v>0.1858672268221308</v>
-      </c>
-      <c r="H20">
+        <v>0.16350237593730055</v>
+      </c>
+      <c r="H30">
         <f t="shared" si="1"/>
-        <v>0.17955668670304584</v>
-      </c>
-      <c r="I20">
+        <v>0.16198663549253883</v>
+      </c>
+      <c r="I30">
         <f t="shared" si="1"/>
-        <v>0.11577247997386925</v>
-      </c>
-      <c r="J20">
+        <v>0.10287785552166615</v>
+      </c>
+      <c r="J30">
         <f t="shared" si="1"/>
-        <v>0.15005602432716975</v>
-      </c>
-      <c r="K20">
+        <v>0.13410975646617768</v>
+      </c>
+      <c r="K30">
         <f t="shared" si="1"/>
-        <v>7.7230105868523913E-2</v>
-      </c>
-      <c r="L20">
+        <v>6.6755865585064883E-2</v>
+      </c>
+      <c r="L30">
         <f t="shared" si="1"/>
-        <v>4.9779137908348342E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+        <v>3.9049868128736356E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B21">
-        <f>B20/(SQRT(16))</f>
-        <v>7.9064994610160734E-3</v>
-      </c>
-      <c r="C21">
-        <f t="shared" ref="C21:L21" si="2">C20/(SQRT(16))</f>
-        <v>3.071749563044536E-2</v>
-      </c>
-      <c r="D21">
+      <c r="B31">
+        <f>B30/SQRT(25)</f>
+        <v>5.6924111618530861E-3</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ref="C31:L31" si="2">C30/SQRT(25)</f>
+        <v>2.2424581133923767E-2</v>
+      </c>
+      <c r="D31">
         <f t="shared" si="2"/>
-        <v>1.7550038377395553E-2</v>
-      </c>
-      <c r="E21">
+        <v>1.2500983377103337E-2</v>
+      </c>
+      <c r="E31">
         <f t="shared" si="2"/>
-        <v>4.5785683846498164E-2</v>
-      </c>
-      <c r="F21">
+        <v>3.2164829213667666E-2</v>
+      </c>
+      <c r="F31">
         <f t="shared" si="2"/>
-        <v>3.3888036283384201E-2</v>
-      </c>
-      <c r="G21">
+        <v>2.4494998639777586E-2</v>
+      </c>
+      <c r="G31">
         <f t="shared" si="2"/>
-        <v>4.6466806705532701E-2</v>
-      </c>
-      <c r="H21">
+        <v>3.270047518746011E-2</v>
+      </c>
+      <c r="H31">
         <f t="shared" si="2"/>
-        <v>4.4889171675761459E-2</v>
-      </c>
-      <c r="I21">
+        <v>3.2397327098507768E-2</v>
+      </c>
+      <c r="I31">
         <f t="shared" si="2"/>
-        <v>2.8943119993467312E-2</v>
-      </c>
-      <c r="J21">
+        <v>2.057557110433323E-2</v>
+      </c>
+      <c r="J31">
         <f t="shared" si="2"/>
-        <v>3.7514006081792436E-2</v>
-      </c>
-      <c r="K21">
+        <v>2.6821951293235537E-2</v>
+      </c>
+      <c r="K31">
         <f t="shared" si="2"/>
-        <v>1.9307526467130978E-2</v>
-      </c>
-      <c r="L21">
+        <v>1.3351173117012977E-2</v>
+      </c>
+      <c r="L31">
         <f t="shared" si="2"/>
-        <v>1.2444784477087086E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+        <v>7.8099736257472713E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B22">
-        <f>B21*1.96</f>
-        <v>1.5496738943591503E-2</v>
-      </c>
-      <c r="C22">
-        <f t="shared" ref="C22:L22" si="3">C21*1.96</f>
-        <v>6.0206291435672903E-2</v>
-      </c>
-      <c r="D22">
+      <c r="B32">
+        <f>B31*1.96</f>
+        <v>1.1157125877232048E-2</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ref="C32:L32" si="3">C31*1.96</f>
+        <v>4.395217902249058E-2</v>
+      </c>
+      <c r="D32">
         <f t="shared" si="3"/>
-        <v>3.4398075219695283E-2</v>
-      </c>
-      <c r="E22">
+        <v>2.4501927419122538E-2</v>
+      </c>
+      <c r="E32">
         <f t="shared" si="3"/>
-        <v>8.9739940339136404E-2</v>
-      </c>
-      <c r="F22">
+        <v>6.3043065258788625E-2</v>
+      </c>
+      <c r="F32">
         <f t="shared" si="3"/>
-        <v>6.6420551115433032E-2</v>
-      </c>
-      <c r="G22">
+        <v>4.8010197333964069E-2</v>
+      </c>
+      <c r="G32">
         <f t="shared" si="3"/>
-        <v>9.107494114284409E-2</v>
-      </c>
-      <c r="H22">
+        <v>6.4092931367421807E-2</v>
+      </c>
+      <c r="H32">
         <f t="shared" si="3"/>
-        <v>8.7982776484492459E-2</v>
-      </c>
-      <c r="I22">
+        <v>6.3498761113075231E-2</v>
+      </c>
+      <c r="I32">
         <f t="shared" si="3"/>
-        <v>5.6728515187195933E-2</v>
-      </c>
-      <c r="J22">
+        <v>4.0328119364493133E-2</v>
+      </c>
+      <c r="J32">
         <f t="shared" si="3"/>
-        <v>7.352745192031318E-2</v>
-      </c>
-      <c r="K22">
+        <v>5.2571024534741648E-2</v>
+      </c>
+      <c r="K32">
         <f t="shared" si="3"/>
-        <v>3.7842751875576716E-2</v>
-      </c>
-      <c r="L22">
+        <v>2.6168299309345434E-2</v>
+      </c>
+      <c r="L32">
         <f t="shared" si="3"/>
-        <v>2.4391777575090687E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+        <v>1.5307548306464651E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B23">
-        <f>B19+B22</f>
-        <v>5.0389017205209802E-2</v>
-      </c>
-      <c r="C23">
-        <f t="shared" ref="C23:L23" si="4">C19+C22</f>
-        <v>0.15711413016573395</v>
-      </c>
-      <c r="D23">
+      <c r="B33">
+        <f>B29+B32</f>
+        <v>4.4790228375898668E-2</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ref="C33:L33" si="4">C29+C32</f>
+        <v>0.13154314616709387</v>
+      </c>
+      <c r="D33">
         <f t="shared" si="4"/>
-        <v>0.10029813371553506</v>
-      </c>
-      <c r="E23">
+        <v>8.5113962240757485E-2</v>
+      </c>
+      <c r="E33">
         <f t="shared" si="4"/>
-        <v>0.30179544219782073</v>
-      </c>
-      <c r="F23">
+        <v>0.23115131282035112</v>
+      </c>
+      <c r="F33">
         <f t="shared" si="4"/>
-        <v>0.21883724881000544</v>
-      </c>
-      <c r="G23">
+        <v>0.16226470129853682</v>
+      </c>
+      <c r="G33">
         <f t="shared" si="4"/>
-        <v>0.28543969524120483</v>
-      </c>
-      <c r="H23">
+        <v>0.21339699731166559</v>
+      </c>
+      <c r="H33">
         <f t="shared" si="4"/>
-        <v>0.26714726426736285</v>
-      </c>
-      <c r="I23">
+        <v>0.19462265500912454</v>
+      </c>
+      <c r="I33">
         <f t="shared" si="4"/>
-        <v>0.14324515438592858</v>
-      </c>
-      <c r="J23">
+        <v>9.3970588507430966E-2</v>
+      </c>
+      <c r="J33">
         <f t="shared" si="4"/>
-        <v>0.18679188120734391</v>
-      </c>
-      <c r="K23">
+        <v>0.12308288360915608</v>
+      </c>
+      <c r="K33">
         <f t="shared" si="4"/>
-        <v>9.748155603968868E-2</v>
-      </c>
-      <c r="L23">
+        <v>8.0022042906335147E-2</v>
+      </c>
+      <c r="L33">
         <f t="shared" si="4"/>
-        <v>3.9592043890580964E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+        <v>3.3487720354659113E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B24">
-        <f>B19-B22</f>
-        <v>1.9395539318026799E-2</v>
-      </c>
-      <c r="C24">
-        <f t="shared" ref="C24:L24" si="5">C19-C22</f>
-        <v>3.6701547294388133E-2</v>
-      </c>
-      <c r="D24">
+      <c r="B34">
+        <f>B29-B32</f>
+        <v>2.2475976621434572E-2</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:L34" si="5">C29-C32</f>
+        <v>4.3638788122112714E-2</v>
+      </c>
+      <c r="D34">
         <f t="shared" si="5"/>
-        <v>3.1501983276144487E-2</v>
-      </c>
-      <c r="E24">
+        <v>3.6110107402512415E-2</v>
+      </c>
+      <c r="E34">
         <f t="shared" si="5"/>
-        <v>0.12231556151954792</v>
-      </c>
-      <c r="F24">
+        <v>0.10506518230277385</v>
+      </c>
+      <c r="F34">
         <f t="shared" si="5"/>
-        <v>8.5996146579139357E-2</v>
-      </c>
-      <c r="G24">
+        <v>6.6244306630608693E-2</v>
+      </c>
+      <c r="G34">
         <f t="shared" si="5"/>
-        <v>0.10328981295551667</v>
-      </c>
-      <c r="H24">
+        <v>8.5211134576821973E-2</v>
+      </c>
+      <c r="H34">
         <f t="shared" si="5"/>
-        <v>9.1181711298377932E-2</v>
-      </c>
-      <c r="I24">
+        <v>6.7625132782974079E-2</v>
+      </c>
+      <c r="I34">
         <f t="shared" si="5"/>
-        <v>2.9788124011536715E-2</v>
-      </c>
-      <c r="J24">
+        <v>1.3314349778444701E-2</v>
+      </c>
+      <c r="J34">
         <f t="shared" si="5"/>
-        <v>3.9736977366717552E-2</v>
-      </c>
-      <c r="K24">
+        <v>1.7940834539672781E-2</v>
+      </c>
+      <c r="K34">
         <f t="shared" si="5"/>
-        <v>2.1796052288535248E-2</v>
-      </c>
-      <c r="L24">
+        <v>2.7685444287644283E-2</v>
+      </c>
+      <c r="L34">
         <f t="shared" si="5"/>
-        <v>-9.19151125960041E-3</v>
+        <v>2.8726237417298125E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1469,15 +1811,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B98B6F23-48BD-402D-A17B-4A837A297F6B}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1515,7 +1857,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2001</v>
       </c>
@@ -1523,13 +1865,13 @@
         <v>1210.9222222222199</v>
       </c>
       <c r="C2">
-        <v>3747.36</v>
+        <v>3594.1041666666702</v>
       </c>
       <c r="D2">
-        <v>2479.1411111111101</v>
+        <v>2402.5131944444402</v>
       </c>
       <c r="E2">
-        <v>4337.8636363636397</v>
+        <v>4014.2</v>
       </c>
       <c r="F2">
         <v>3296.9333333333302</v>
@@ -1541,19 +1883,19 @@
         <v>2829.125</v>
       </c>
       <c r="I2">
-        <v>817.79222222222199</v>
+        <v>894.42013888888903</v>
       </c>
       <c r="J2">
-        <v>349.983888888889</v>
+        <v>426.61180555555597</v>
       </c>
       <c r="K2">
-        <v>1040.9303030302999</v>
+        <v>717.26666666666597</v>
       </c>
       <c r="L2">
         <v>537.32327586206895</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2002</v>
       </c>
@@ -1567,7 +1909,7 @@
         <v>982.19460049937595</v>
       </c>
       <c r="E3">
-        <v>4019.28947368421</v>
+        <v>3610.2058823529401</v>
       </c>
       <c r="F3">
         <v>3008.8085106383</v>
@@ -1585,24 +1927,24 @@
         <v>223.54825664348101</v>
       </c>
       <c r="K3">
-        <v>1010.48096304591</v>
+        <v>601.39737171464299</v>
       </c>
       <c r="L3">
         <v>47.846886446886401</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2003</v>
       </c>
       <c r="B4">
-        <v>2891.2048192771099</v>
+        <v>2778.0123456790102</v>
       </c>
       <c r="C4">
-        <v>2229.0714285714298</v>
+        <v>2099.2682926829302</v>
       </c>
       <c r="D4">
-        <v>2560.1381239242701</v>
+        <v>2438.64031918097</v>
       </c>
       <c r="E4">
         <v>1590.0476190476199</v>
@@ -1617,10 +1959,10 @@
         <v>1347.26829268293</v>
       </c>
       <c r="I4">
-        <v>-833.554790590935</v>
+        <v>-712.05698584763604</v>
       </c>
       <c r="J4">
-        <v>-1212.8698312413401</v>
+        <v>-1091.37202649804</v>
       </c>
       <c r="K4">
         <v>-136.53571428571399</v>
@@ -1629,7 +1971,7 @@
         <v>-48.979403794037999</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2004</v>
       </c>
@@ -1637,13 +1979,13 @@
         <v>943.02150537634395</v>
       </c>
       <c r="C5">
-        <v>743.378947368421</v>
+        <v>673.20212765957399</v>
       </c>
       <c r="D5">
-        <v>843.20022637238299</v>
+        <v>808.11181651795903</v>
       </c>
       <c r="E5">
-        <v>2442.0392156862699</v>
+        <v>2336.8200000000002</v>
       </c>
       <c r="F5">
         <v>2373.9074074074101</v>
@@ -1655,19 +1997,19 @@
         <v>2271.8909090909101</v>
       </c>
       <c r="I5">
-        <v>1530.7071810350201</v>
+        <v>1565.7955908894501</v>
       </c>
       <c r="J5">
-        <v>1428.6906827185301</v>
+        <v>1463.77909257295</v>
       </c>
       <c r="K5">
-        <v>68.131808278867098</v>
+        <v>-37.087407407407198</v>
       </c>
       <c r="L5">
         <v>265.84983164983203</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2006</v>
       </c>
@@ -1705,7 +2047,7 @@
         <v>763.87779433680998</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2007</v>
       </c>
@@ -1719,7 +2061,7 @@
         <v>1465.6224560592</v>
       </c>
       <c r="E7">
-        <v>3206.5370370370401</v>
+        <v>3047.6346153846198</v>
       </c>
       <c r="F7">
         <v>3060.1111111111099</v>
@@ -1737,13 +2079,13 @@
         <v>1274.7775439407999</v>
       </c>
       <c r="K7">
-        <v>146.42592592592601</v>
+        <v>-12.476495726496101</v>
       </c>
       <c r="L7">
         <v>143.255737704918</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2009</v>
       </c>
@@ -1781,7 +2123,7 @@
         <v>-88.508771929824704</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2010</v>
       </c>
@@ -1819,7 +2161,7 @@
         <v>-82.295238095238105</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2011</v>
       </c>
@@ -1833,13 +2175,13 @@
         <v>1308.3693181818201</v>
       </c>
       <c r="E10">
-        <v>3321.8372093023299</v>
+        <v>3221.2142857142899</v>
       </c>
       <c r="F10">
         <v>2962.3181818181802</v>
       </c>
       <c r="G10">
-        <v>2752.5636363636399</v>
+        <v>2661.5925925925899</v>
       </c>
       <c r="H10">
         <v>2562.4827586206902</v>
@@ -1851,13 +2193,13 @@
         <v>1254.1134404388699</v>
       </c>
       <c r="K10">
-        <v>359.51902748414301</v>
+        <v>258.89610389610402</v>
       </c>
       <c r="L10">
-        <v>190.080877742947</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>99.109833971902802</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2012</v>
       </c>
@@ -1895,7 +2237,7 @@
         <v>406.03947368421098</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -1933,7 +2275,7 @@
         <v>-11.816280384397899</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -1971,7 +2313,7 @@
         <v>-28.339080459770098</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2017</v>
       </c>
@@ -1988,7 +2330,7 @@
         <v>1876.60377358491</v>
       </c>
       <c r="F14">
-        <v>1961.7966101694899</v>
+        <v>1868.3275862068999</v>
       </c>
       <c r="G14">
         <v>1814.7</v>
@@ -1997,19 +2339,19 @@
         <v>1670.6071428571399</v>
       </c>
       <c r="I14">
-        <v>1056.6462441205299</v>
+        <v>963.17722015793697</v>
       </c>
       <c r="J14">
         <v>765.45677680818403</v>
       </c>
       <c r="K14">
-        <v>-85.192836584585805</v>
+        <v>8.27618737800913</v>
       </c>
       <c r="L14">
         <v>144.09285714285701</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2019</v>
       </c>
@@ -2047,7 +2389,7 @@
         <v>653.95735849056598</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2020</v>
       </c>
@@ -2085,336 +2427,678 @@
         <v>-29.298534798534799</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
+        <v>2021</v>
+      </c>
+      <c r="B17">
+        <v>1299.4631578947401</v>
+      </c>
+      <c r="C17">
+        <v>1650.7101449275401</v>
+      </c>
+      <c r="D17">
+        <v>1475.0866514111401</v>
+      </c>
+      <c r="E17">
+        <v>2693.4166666666702</v>
+      </c>
+      <c r="F17">
+        <v>2745.5294117647099</v>
+      </c>
+      <c r="G17">
+        <v>2608.9387755101998</v>
+      </c>
+      <c r="H17">
+        <v>2206.7058823529401</v>
+      </c>
+      <c r="I17">
+        <v>1270.4427603535701</v>
+      </c>
+      <c r="J17">
+        <v>731.61923094180395</v>
+      </c>
+      <c r="K17">
+        <v>-52.112745098039298</v>
+      </c>
+      <c r="L17">
+        <v>402.23289315726299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2022</v>
+      </c>
+      <c r="B18">
+        <v>903.21052631578902</v>
+      </c>
+      <c r="C18">
+        <v>847.659574468085</v>
+      </c>
+      <c r="D18">
+        <v>875.43505039193701</v>
+      </c>
+      <c r="E18">
+        <v>2085.8363636363601</v>
+      </c>
+      <c r="F18">
+        <v>2208.8474576271201</v>
+      </c>
+      <c r="G18">
+        <v>2428.43103448276</v>
+      </c>
+      <c r="H18">
+        <v>2260.2931034482799</v>
+      </c>
+      <c r="I18">
+        <v>1333.4124072351799</v>
+      </c>
+      <c r="J18">
+        <v>1384.8580530563399</v>
+      </c>
+      <c r="K18">
+        <v>-123.011093990755</v>
+      </c>
+      <c r="L18">
+        <v>168.13793103448299</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>2023</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <v>794.627659574468</v>
       </c>
-      <c r="C17">
+      <c r="C19">
         <v>846.531914893617</v>
       </c>
-      <c r="D17">
+      <c r="D19">
         <v>820.57978723404301</v>
       </c>
-      <c r="E17">
+      <c r="E19">
+        <v>1639.0925925925901</v>
+      </c>
+      <c r="F19">
+        <v>1532.46551724138</v>
+      </c>
+      <c r="G19">
         <v>1706.2758620689699</v>
       </c>
-      <c r="F17">
+      <c r="H19">
         <v>1838.1803278688501</v>
       </c>
-      <c r="G17">
-        <v>1639.0925925925901</v>
-      </c>
-      <c r="H17">
-        <v>1532.46551724138</v>
-      </c>
-      <c r="I17">
+      <c r="I19">
+        <v>711.88573000733697</v>
+      </c>
+      <c r="J19">
         <v>1017.60054063481</v>
       </c>
-      <c r="J17">
-        <v>711.88573000733697</v>
-      </c>
-      <c r="K17">
+      <c r="K19">
+        <v>106.62707535121299</v>
+      </c>
+      <c r="L19">
         <v>-131.90446579988699</v>
       </c>
-      <c r="L17">
-        <v>106.62707535121299</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2024</v>
+      </c>
+      <c r="B20">
+        <v>982.52808988764002</v>
+      </c>
+      <c r="C20">
+        <v>1053.2195121951199</v>
+      </c>
+      <c r="D20">
+        <v>1017.87380104138</v>
+      </c>
+      <c r="E20">
+        <v>3377.4423076923099</v>
+      </c>
+      <c r="F20">
+        <v>2252.8448275862102</v>
+      </c>
+      <c r="G20">
+        <v>2997.6666666666702</v>
+      </c>
+      <c r="H20">
+        <v>2335.8913043478301</v>
+      </c>
+      <c r="I20">
+        <v>1234.97102654483</v>
+      </c>
+      <c r="J20">
+        <v>1318.0175033064399</v>
+      </c>
+      <c r="K20">
+        <v>1124.5974801061</v>
+      </c>
+      <c r="L20">
+        <v>661.77536231884096</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2025</v>
+      </c>
+      <c r="B21">
+        <v>971.06315789473695</v>
+      </c>
+      <c r="C21">
+        <v>760.15053763440903</v>
+      </c>
+      <c r="D21">
+        <v>865.60684776457299</v>
+      </c>
+      <c r="E21">
+        <v>2518.76923076923</v>
+      </c>
+      <c r="F21">
+        <v>2813.56896551724</v>
+      </c>
+      <c r="G21">
+        <v>2224.7049180327899</v>
+      </c>
+      <c r="H21">
+        <v>2487.3571428571399</v>
+      </c>
+      <c r="I21">
+        <v>1947.9621177526701</v>
+      </c>
+      <c r="J21">
+        <v>1621.75029509257</v>
+      </c>
+      <c r="K21">
+        <v>-294.79973474801</v>
+      </c>
+      <c r="L21">
+        <v>-262.65222482435598</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2026</v>
+      </c>
+      <c r="B22">
+        <v>800.81521739130403</v>
+      </c>
+      <c r="C22">
+        <v>1213.27659574468</v>
+      </c>
+      <c r="D22">
+        <v>1007.04590656799</v>
+      </c>
+      <c r="E22">
+        <v>2123.75</v>
+      </c>
+      <c r="F22">
+        <v>1690.0892857142901</v>
+      </c>
+      <c r="G22">
+        <v>2379.06896551724</v>
+      </c>
+      <c r="H22">
+        <v>1446.7719298245599</v>
+      </c>
+      <c r="I22">
+        <v>683.04337914629298</v>
+      </c>
+      <c r="J22">
+        <v>439.72602325656902</v>
+      </c>
+      <c r="K22">
+        <v>433.66071428571399</v>
+      </c>
+      <c r="L22">
+        <v>932.29703569267997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2027</v>
+      </c>
+      <c r="B23">
+        <v>1336.38709677419</v>
+      </c>
+      <c r="C23">
+        <v>1750.8571428571399</v>
+      </c>
+      <c r="D23">
+        <v>1543.62211981567</v>
+      </c>
+      <c r="E23">
+        <v>3600.8392857142899</v>
+      </c>
+      <c r="F23">
+        <v>3577.1636363636399</v>
+      </c>
+      <c r="G23">
+        <v>3112.3928571428601</v>
+      </c>
+      <c r="H23">
+        <v>2839.5438596491199</v>
+      </c>
+      <c r="I23">
+        <v>2033.5415165479701</v>
+      </c>
+      <c r="J23">
+        <v>1295.9217398334499</v>
+      </c>
+      <c r="K23">
+        <v>23.6756493506496</v>
+      </c>
+      <c r="L23">
+        <v>272.848997493735</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2028</v>
+      </c>
+      <c r="B24">
+        <v>1018.64444444444</v>
+      </c>
+      <c r="C24">
+        <v>899.03157894736796</v>
+      </c>
+      <c r="D24">
+        <v>958.83801169590595</v>
+      </c>
+      <c r="E24">
+        <v>2314.4464285714298</v>
+      </c>
+      <c r="F24">
+        <v>2039.82456140351</v>
+      </c>
+      <c r="G24">
+        <v>2018.8392857142901</v>
+      </c>
+      <c r="H24">
+        <v>1958.0333333333299</v>
+      </c>
+      <c r="I24">
+        <v>1080.9865497076</v>
+      </c>
+      <c r="J24">
+        <v>999.19532163742701</v>
+      </c>
+      <c r="K24">
+        <v>274.62186716792002</v>
+      </c>
+      <c r="L24">
+        <v>60.805952380952498</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2029</v>
+      </c>
+      <c r="B25">
+        <v>905.04301075268802</v>
+      </c>
+      <c r="C25">
+        <v>1139.2159090909099</v>
+      </c>
+      <c r="D25">
+        <v>1022.1294599218</v>
+      </c>
+      <c r="E25">
+        <v>2619.8518518518499</v>
+      </c>
+      <c r="F25">
+        <v>2456.0909090909099</v>
+      </c>
+      <c r="G25">
+        <v>2066.3157894736801</v>
+      </c>
+      <c r="H25">
+        <v>1794.91379310345</v>
+      </c>
+      <c r="I25">
+        <v>1433.96144916911</v>
+      </c>
+      <c r="J25">
+        <v>772.78433318165003</v>
+      </c>
+      <c r="K25">
+        <v>163.76094276094301</v>
+      </c>
+      <c r="L25">
+        <v>271.40199637023602</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2031</v>
+      </c>
+      <c r="B26">
+        <v>886.89361702127701</v>
+      </c>
+      <c r="C26">
+        <v>853.659574468085</v>
+      </c>
+      <c r="D26">
+        <v>870.276595744681</v>
+      </c>
+      <c r="E26">
+        <v>2083.6666666666702</v>
+      </c>
+      <c r="F26">
+        <v>1800.63333333333</v>
+      </c>
+      <c r="G26">
+        <v>1957.3793103448299</v>
+      </c>
+      <c r="H26">
+        <v>1665.53448275862</v>
+      </c>
+      <c r="I26">
+        <v>930.356737588653</v>
+      </c>
+      <c r="J26">
+        <v>795.25788701394004</v>
+      </c>
+      <c r="K26">
+        <v>283.03333333333302</v>
+      </c>
+      <c r="L26">
+        <v>291.84482758620697</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B19">
-        <f t="shared" ref="B19:L19" si="0">AVERAGE(B2:B17)</f>
-        <v>1146.146186976194</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>1306.8967937964485</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>1226.5214903863209</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>2054.8929362414237</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>1926.9166400181368</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="0"/>
-        <v>1864.3510720103288</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="0"/>
-        <v>1678.7439558259227</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="0"/>
-        <v>700.39514963181568</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="0"/>
-        <v>452.22246543960205</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="0"/>
-        <v>127.97629622328475</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="0"/>
-        <v>185.60711618440661</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="B29">
+        <f>AVERAGE(B2:B26)</f>
+        <v>1093.1677934559125</v>
+      </c>
+      <c r="C29">
+        <f>AVERAGE(C2:C26)</f>
+        <v>1228.9957392858335</v>
+      </c>
+      <c r="D29">
+        <f>AVERAGE(D2:D26)</f>
+        <v>1161.0817663708729</v>
+      </c>
+      <c r="E29">
+        <f>AVERAGE(E2:E26)</f>
+        <v>2205.2652289333423</v>
+      </c>
+      <c r="F29">
+        <f>AVERAGE(F2:F26)</f>
+        <v>2080.6429917640435</v>
+      </c>
+      <c r="G29">
+        <f>AVERAGE(G2:G26)</f>
+        <v>2063.9826792302365</v>
+      </c>
+      <c r="H29">
+        <f>AVERAGE(H2:H26)</f>
+        <v>1846.4265174207001</v>
+      </c>
+      <c r="I29">
+        <f>AVERAGE(I2:I26)</f>
+        <v>919.56122539317028</v>
+      </c>
+      <c r="J29">
+        <f>AVERAGE(J2:J26)</f>
+        <v>685.34475104982732</v>
+      </c>
+      <c r="K29">
+        <f>AVERAGE(K2:K26)</f>
+        <v>124.62223716929877</v>
+      </c>
+      <c r="L29">
+        <f>AVERAGE(L2:L26)</f>
+        <v>217.55616180953606</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B20">
-        <f t="shared" ref="B20:L20" si="1">STDEV(B2:B17)</f>
-        <v>510.44405814454018</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="1"/>
-        <v>765.58445990244127</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="1"/>
-        <v>555.73419778473431</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="1"/>
-        <v>1138.6588263577223</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="1"/>
-        <v>844.36349953521778</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="1"/>
-        <v>797.03591879638589</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="1"/>
-        <v>641.57021397072299</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="1"/>
-        <v>826.24216688807178</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="1"/>
-        <v>661.03632158600533</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="1"/>
-        <v>381.22218054840783</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="1"/>
-        <v>270.07539130458628</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B30">
+        <f>STDEV(B2:B26)</f>
+        <v>402.74475030275539</v>
+      </c>
+      <c r="C30">
+        <f>STDEV(C2:C26)</f>
+        <v>614.9237631376202</v>
+      </c>
+      <c r="D30">
+        <f>STDEV(D2:D26)</f>
+        <v>447.50149847505719</v>
+      </c>
+      <c r="E30">
+        <f>STDEV(E2:E26)</f>
+        <v>926.92046292609007</v>
+      </c>
+      <c r="F30">
+        <f>STDEV(F2:F26)</f>
+        <v>790.13452017962175</v>
+      </c>
+      <c r="G30">
+        <f>STDEV(G2:G26)</f>
+        <v>722.73504954824682</v>
+      </c>
+      <c r="H30">
+        <f>STDEV(H2:H26)</f>
+        <v>601.07031883664899</v>
+      </c>
+      <c r="I30">
+        <f>STDEV(I2:I26)</f>
+        <v>755.19378897561819</v>
+      </c>
+      <c r="J30">
+        <f>STDEV(J2:J26)</f>
+        <v>626.33488343409249</v>
+      </c>
+      <c r="K30">
+        <f>STDEV(K2:K26)</f>
+        <v>320.52814715776873</v>
+      </c>
+      <c r="L30">
+        <f>STDEV(L2:L26)</f>
+        <v>305.83994998619454</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B21">
-        <f t="shared" ref="B21:L21" si="2">B20/(SQRT(16))</f>
-        <v>127.61101453613504</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="2"/>
-        <v>191.39611497561032</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="2"/>
-        <v>138.93354944618358</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="2"/>
-        <v>284.66470658943058</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="2"/>
-        <v>211.09087488380445</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="2"/>
-        <v>199.25897969909647</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="2"/>
-        <v>160.39255349268075</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="2"/>
-        <v>206.56054172201794</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="2"/>
-        <v>165.25908039650133</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="2"/>
-        <v>95.305545137101959</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="2"/>
-        <v>67.518847826146569</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="B31">
+        <f>B30/SQRT(25)</f>
+        <v>80.548950060551078</v>
+      </c>
+      <c r="C31">
+        <f>C30/SQRT(25)</f>
+        <v>122.98475262752405</v>
+      </c>
+      <c r="D31">
+        <f>D30/SQRT(25)</f>
+        <v>89.500299695011435</v>
+      </c>
+      <c r="E31">
+        <f>E30/SQRT(25)</f>
+        <v>185.38409258521801</v>
+      </c>
+      <c r="F31">
+        <f>F30/SQRT(25)</f>
+        <v>158.02690403592436</v>
+      </c>
+      <c r="G31">
+        <f>G30/SQRT(25)</f>
+        <v>144.54700990964938</v>
+      </c>
+      <c r="H31">
+        <f>H30/SQRT(25)</f>
+        <v>120.2140637673298</v>
+      </c>
+      <c r="I31">
+        <f>I30/SQRT(25)</f>
+        <v>151.03875779512364</v>
+      </c>
+      <c r="J31">
+        <f>J30/SQRT(25)</f>
+        <v>125.2669766868185</v>
+      </c>
+      <c r="K31">
+        <f>K30/SQRT(25)</f>
+        <v>64.105629431553751</v>
+      </c>
+      <c r="L31">
+        <f>L30/SQRT(25)</f>
+        <v>61.167989997238905</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B22">
-        <f t="shared" ref="B22:L22" si="3">B21*1.96</f>
-        <v>250.11758849082469</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="3"/>
-        <v>375.13638535219621</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="3"/>
-        <v>272.30975691451982</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="3"/>
-        <v>557.94282491528395</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="3"/>
-        <v>413.73811477225672</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="3"/>
-        <v>390.54760021022906</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="3"/>
-        <v>314.36940484565423</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="3"/>
-        <v>404.85866177515516</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="3"/>
-        <v>323.90779757714262</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="3"/>
-        <v>186.79886846871983</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="3"/>
-        <v>132.33694173924727</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B32">
+        <f>B31*1.96</f>
+        <v>157.87594211868011</v>
+      </c>
+      <c r="C32">
+        <f>C31*1.96</f>
+        <v>241.05011514994712</v>
+      </c>
+      <c r="D32">
+        <f>D31*1.96</f>
+        <v>175.42058740222242</v>
+      </c>
+      <c r="E32">
+        <f>E31*1.96</f>
+        <v>363.3528214670273</v>
+      </c>
+      <c r="F32">
+        <f>F31*1.96</f>
+        <v>309.73273191041176</v>
+      </c>
+      <c r="G32">
+        <f>G31*1.96</f>
+        <v>283.31213942291276</v>
+      </c>
+      <c r="H32">
+        <f>H31*1.96</f>
+        <v>235.6195649839664</v>
+      </c>
+      <c r="I32">
+        <f>I31*1.96</f>
+        <v>296.03596527844235</v>
+      </c>
+      <c r="J32">
+        <f>J31*1.96</f>
+        <v>245.52327430616424</v>
+      </c>
+      <c r="K32">
+        <f>K31*1.96</f>
+        <v>125.64703368584534</v>
+      </c>
+      <c r="L32">
+        <f>L31*1.96</f>
+        <v>119.88926039458825</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B23">
-        <f t="shared" ref="B23:L23" si="4">B19+B22</f>
-        <v>1396.2637754670186</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="4"/>
-        <v>1682.0331791486446</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="4"/>
-        <v>1498.8312473008407</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="4"/>
-        <v>2612.8357611567076</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="4"/>
-        <v>2340.6547547903938</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="4"/>
-        <v>2254.8986722205577</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="4"/>
-        <v>1993.1133606715771</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="4"/>
-        <v>1105.2538114069707</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="4"/>
-        <v>776.13026301674472</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="4"/>
-        <v>314.77516469200458</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="4"/>
-        <v>317.94405792365387</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B33">
+        <f>B29+B32</f>
+        <v>1251.0437355745926</v>
+      </c>
+      <c r="C33">
+        <f>C29+C32</f>
+        <v>1470.0458544357805</v>
+      </c>
+      <c r="D33">
+        <f>D29+D32</f>
+        <v>1336.5023537730954</v>
+      </c>
+      <c r="E33">
+        <f>E29+E32</f>
+        <v>2568.6180504003696</v>
+      </c>
+      <c r="F33">
+        <f>F29+F32</f>
+        <v>2390.375723674455</v>
+      </c>
+      <c r="G33">
+        <f>G29+G32</f>
+        <v>2347.2948186531494</v>
+      </c>
+      <c r="H33">
+        <f>H29+H32</f>
+        <v>2082.0460824046663</v>
+      </c>
+      <c r="I33">
+        <f>I29+I32</f>
+        <v>1215.5971906716127</v>
+      </c>
+      <c r="J33">
+        <f>J29+J32</f>
+        <v>930.86802535599156</v>
+      </c>
+      <c r="K33">
+        <f>K29+K32</f>
+        <v>250.2692708551441</v>
+      </c>
+      <c r="L33">
+        <f>L29+L32</f>
+        <v>337.44542220412433</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B24">
-        <f t="shared" ref="B24:K24" si="5">B19-B22</f>
-        <v>896.02859848536934</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="5"/>
-        <v>931.76040844425233</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="5"/>
-        <v>954.21173347180115</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="5"/>
-        <v>1496.9501113261399</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="5"/>
-        <v>1513.1785252458801</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="5"/>
-        <v>1473.8034718000997</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="5"/>
-        <v>1364.3745509802684</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="5"/>
-        <v>295.53648785666053</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="5"/>
-        <v>128.31466786245943</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="5"/>
-        <v>-58.822572245435083</v>
-      </c>
-      <c r="L24">
-        <f t="shared" ref="L24" si="6">L19-L22</f>
-        <v>53.270174445159341</v>
+      <c r="B34">
+        <f>B29-B32</f>
+        <v>935.2918513372324</v>
+      </c>
+      <c r="C34">
+        <f>C29-C32</f>
+        <v>987.94562413588631</v>
+      </c>
+      <c r="D34">
+        <f>D29-D32</f>
+        <v>985.66117896865046</v>
+      </c>
+      <c r="E34">
+        <f>E29-E32</f>
+        <v>1841.912407466315</v>
+      </c>
+      <c r="F34">
+        <f>F29-F32</f>
+        <v>1770.9102598536317</v>
+      </c>
+      <c r="G34">
+        <f>G29-G32</f>
+        <v>1780.6705398073236</v>
+      </c>
+      <c r="H34">
+        <f>H29-H32</f>
+        <v>1610.8069524367336</v>
+      </c>
+      <c r="I34">
+        <f>I29-I32</f>
+        <v>623.52526011472787</v>
+      </c>
+      <c r="J34">
+        <f>J29-J32</f>
+        <v>439.82147674366308</v>
+      </c>
+      <c r="K34">
+        <f>K29-K32</f>
+        <v>-1.0247965165465729</v>
+      </c>
+      <c r="L34">
+        <f>L29-L32</f>
+        <v>97.666901414947816</v>
       </c>
     </row>
   </sheetData>
@@ -2424,15 +3108,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B5B3B6-E066-499C-A3AA-C3C7E4C73E0C}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2470,884 +3154,1248 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2001</v>
       </c>
       <c r="B2">
-        <v>-0.26334776681299898</v>
+        <v>-0.27092930299071799</v>
       </c>
       <c r="C2">
-        <v>0.99666205516185602</v>
+        <v>1.05649728678726</v>
       </c>
       <c r="D2">
-        <v>0.36665714417442802</v>
+        <v>0.39278399189827101</v>
       </c>
       <c r="E2">
-        <v>1.29000273485396</v>
+        <v>1.29048965179387</v>
       </c>
       <c r="F2">
-        <v>0.77290650749901202</v>
+        <v>0.89097385002544705</v>
       </c>
       <c r="G2">
-        <v>0.807438996774962</v>
+        <v>0.92969350519682004</v>
       </c>
       <c r="H2">
-        <v>0.54051638148610104</v>
+        <v>0.63040573770234598</v>
       </c>
       <c r="I2">
-        <v>0.406249363324584</v>
+        <v>0.49818985812717498</v>
       </c>
       <c r="J2">
-        <v>0.17385923731167299</v>
+        <v>0.237621745804074</v>
       </c>
       <c r="K2">
-        <v>0.51709622735494398</v>
+        <v>0.399515801768422</v>
       </c>
       <c r="L2">
-        <v>0.26692261528886102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.299287767494474</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2002</v>
       </c>
       <c r="B3">
-        <v>-0.44734606901156998</v>
+        <v>-0.47723794052669199</v>
       </c>
       <c r="C3">
-        <v>-0.306596552993811</v>
+        <v>-0.31942213170398798</v>
       </c>
       <c r="D3">
-        <v>-0.37697131100269099</v>
+        <v>-0.39833003611534001</v>
       </c>
       <c r="E3">
-        <v>1.1317467044792699</v>
+        <v>1.06546590355311</v>
       </c>
       <c r="F3">
-        <v>0.62977659919565299</v>
+        <v>0.73048901935104604</v>
       </c>
       <c r="G3">
-        <v>-0.24215209764523399</v>
+        <v>-0.24716359659335299</v>
       </c>
       <c r="H3">
-        <v>-0.265920686570294</v>
+        <v>-0.27381419683633601</v>
       </c>
       <c r="I3">
-        <v>1.0067479101983401</v>
+        <v>1.1288190554663899</v>
       </c>
       <c r="J3">
-        <v>0.11105062443239599</v>
+        <v>0.124515839279004</v>
       </c>
       <c r="K3">
-        <v>0.50197010528361896</v>
+        <v>0.33497688420206101</v>
       </c>
       <c r="L3">
-        <v>2.37685889250598E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.6650600242983401E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2003</v>
       </c>
       <c r="B4">
-        <v>0.57135537257860503</v>
+        <v>0.60193611263742997</v>
       </c>
       <c r="C4">
-        <v>0.24243164219732399</v>
+        <v>0.22387731368546401</v>
       </c>
       <c r="D4">
-        <v>0.40689350738796498</v>
+        <v>0.412906713161447</v>
       </c>
       <c r="E4">
-        <v>-7.5012090714278695E-2</v>
+        <v>-5.9757372211644497E-2</v>
       </c>
       <c r="F4">
-        <v>-7.18612527661012E-3</v>
+        <v>1.62926910324507E-2</v>
       </c>
       <c r="G4">
-        <v>-0.219947191771238</v>
+        <v>-0.22226628057064901</v>
       </c>
       <c r="H4">
-        <v>-0.19561600951411601</v>
+        <v>-0.194984870899331</v>
       </c>
       <c r="I4">
-        <v>-0.41407963266457498</v>
+        <v>-0.39661402212899599</v>
       </c>
       <c r="J4">
-        <v>-0.60250951690208099</v>
+        <v>-0.60789158406077803</v>
       </c>
       <c r="K4">
-        <v>-6.7825965437668598E-2</v>
+        <v>-7.6050063244095106E-2</v>
       </c>
       <c r="L4">
-        <v>-2.43311822571219E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>-2.72814096713185E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2004</v>
       </c>
       <c r="B5">
-        <v>-0.39643107660175803</v>
+        <v>-0.420149355530474</v>
       </c>
       <c r="C5">
-        <v>-0.49560622143600602</v>
+        <v>-0.57043809754344799</v>
       </c>
       <c r="D5">
-        <v>-0.446018649018882</v>
+        <v>-0.49529372653696102</v>
       </c>
       <c r="E5">
-        <v>0.34822627507968701</v>
+        <v>0.35619304118370498</v>
       </c>
       <c r="F5">
-        <v>0.31438087647681201</v>
+        <v>0.37685063757632897</v>
       </c>
       <c r="G5">
-        <v>0.39576730392063397</v>
+        <v>0.46810540873033002</v>
       </c>
       <c r="H5">
-        <v>0.26370279913210098</v>
+        <v>0.32002769429369698</v>
       </c>
       <c r="I5">
-        <v>0.76039952549569401</v>
+        <v>0.87214436411328999</v>
       </c>
       <c r="J5">
-        <v>0.70972144815098304</v>
+        <v>0.81532142083065795</v>
       </c>
       <c r="K5">
-        <v>3.3845398602875297E-2</v>
+        <v>-2.06575963926235E-2</v>
       </c>
       <c r="L5">
-        <v>0.13206450478853299</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.14807771443663301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2006</v>
       </c>
       <c r="B6">
-        <v>-0.255997391221504</v>
+        <v>-0.26268767273902899</v>
       </c>
       <c r="C6">
-        <v>-0.20530283487079701</v>
+        <v>-0.20584625232245399</v>
       </c>
       <c r="D6">
-        <v>-0.23065011304615099</v>
+        <v>-0.234266962530742</v>
       </c>
       <c r="E6">
-        <v>0.14929734830115901</v>
+        <v>0.19175024604774299</v>
       </c>
       <c r="F6">
-        <v>0.17823914725969101</v>
+        <v>0.22420132325676501</v>
       </c>
       <c r="G6">
-        <v>0.38883553719962299</v>
+        <v>0.46033314490593003</v>
       </c>
       <c r="H6">
-        <v>9.3688961940907693E-3</v>
+        <v>3.4855057549904297E-2</v>
       </c>
       <c r="I6">
-        <v>0.408889260305842</v>
+        <v>0.45846828578750698</v>
       </c>
       <c r="J6">
-        <v>0.240019009240241</v>
+        <v>0.26912202008064601</v>
       </c>
       <c r="K6">
-        <v>-2.8941798958532199E-2</v>
+        <v>-3.2451077209022502E-2</v>
       </c>
       <c r="L6">
-        <v>0.37946664100553201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.42547808735602599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2007</v>
       </c>
       <c r="B7">
-        <v>-0.194998742617225</v>
+        <v>-0.19429275857561901</v>
       </c>
       <c r="C7">
-        <v>-7.8645208899743094E-2</v>
+        <v>-6.3831016663218901E-2</v>
       </c>
       <c r="D7">
-        <v>-0.13682197575848401</v>
+        <v>-0.129061887619419</v>
       </c>
       <c r="E7">
-        <v>0.72800092290262097</v>
+        <v>0.752115065964025</v>
       </c>
       <c r="F7">
-        <v>0.65526186087048499</v>
+        <v>0.75906444396397599</v>
       </c>
       <c r="G7">
-        <v>0.56760526405586298</v>
+        <v>0.66077922696045999</v>
       </c>
       <c r="H7">
-        <v>0.49644103596248002</v>
+        <v>0.58098612689478402</v>
       </c>
       <c r="I7">
-        <v>0.79208383662896997</v>
+        <v>0.88812633158339505</v>
       </c>
       <c r="J7">
-        <v>0.633263011720964</v>
+        <v>0.71004801451420396</v>
       </c>
       <c r="K7">
-        <v>7.2739062032135801E-2</v>
+        <v>-6.9493779999508804E-3</v>
       </c>
       <c r="L7">
-        <v>7.1164228093382603E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.9793100065675596E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2009</v>
       </c>
       <c r="B8">
-        <v>-0.14750182593896799</v>
+        <v>-0.14103670104702401</v>
       </c>
       <c r="C8">
-        <v>-0.16617724592272901</v>
+        <v>-0.16197657063399301</v>
       </c>
       <c r="D8">
-        <v>-0.15683953593084901</v>
+        <v>-0.151506635840509</v>
       </c>
       <c r="E8">
-        <v>-0.45713607485735303</v>
+        <v>-0.48821501337670498</v>
       </c>
       <c r="F8">
-        <v>-0.38643552256950903</v>
+        <v>-0.408941811171803</v>
       </c>
       <c r="G8">
-        <v>-0.19980618982193299</v>
+        <v>-0.19968312289408399</v>
       </c>
       <c r="H8">
-        <v>-0.155838258520965</v>
+        <v>-0.15038395059961099</v>
       </c>
       <c r="I8">
-        <v>-0.22959598663865999</v>
+        <v>-0.25743517533129401</v>
       </c>
       <c r="J8">
-        <v>1.0012774098832899E-3</v>
+        <v>1.1226852408976499E-3</v>
       </c>
       <c r="K8">
-        <v>-7.0700552287844207E-2</v>
+        <v>-7.9273202204902193E-2</v>
       </c>
       <c r="L8">
-        <v>-4.3967931300967301E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>-4.92991722944729E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2010</v>
       </c>
       <c r="B9">
-        <v>-0.50265835206366205</v>
+        <v>-0.539257000589354</v>
       </c>
       <c r="C9">
-        <v>-0.50154952718924495</v>
+        <v>-0.53801372743751796</v>
       </c>
       <c r="D9">
-        <v>-0.50210393962645306</v>
+        <v>-0.53863536401343604</v>
       </c>
       <c r="E9">
-        <v>-0.52575834249761599</v>
+        <v>-0.56515793280763005</v>
       </c>
       <c r="F9">
-        <v>-0.49196713136203402</v>
+        <v>-0.52726943793147296</v>
       </c>
       <c r="G9">
-        <v>-0.51543318748351796</v>
+        <v>-0.55358082237860395</v>
       </c>
       <c r="H9">
-        <v>-0.47455191327674201</v>
+        <v>-0.507742573429805</v>
       </c>
       <c r="I9">
-        <v>1.0136808264418699E-2</v>
+        <v>1.1365926081962701E-2</v>
       </c>
       <c r="J9">
-        <v>2.7552026349711101E-2</v>
+        <v>3.0892790583631102E-2</v>
       </c>
       <c r="K9">
-        <v>-3.3791211135581298E-2</v>
+        <v>-3.7888494876157197E-2</v>
       </c>
       <c r="L9">
-        <v>-4.0881274206776202E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>-4.5838248948799502E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2011</v>
       </c>
       <c r="B10">
-        <v>-0.32701905428524097</v>
+        <v>-0.34232092134588799</v>
       </c>
       <c r="C10">
-        <v>-0.102860149677358</v>
+        <v>-9.09820902337376E-2</v>
       </c>
       <c r="D10">
-        <v>-0.21493960198129999</v>
+        <v>-0.21665150578981299</v>
       </c>
       <c r="E10">
-        <v>0.78527784520778299</v>
+        <v>0.84879852329619798</v>
       </c>
       <c r="F10">
-        <v>0.60668189864616495</v>
+        <v>0.704594018431286</v>
       </c>
       <c r="G10">
-        <v>0.502483487081679</v>
+        <v>0.53709059121907898</v>
       </c>
       <c r="H10">
-        <v>0.408058236431317</v>
+        <v>0.48188665295936101</v>
       </c>
       <c r="I10">
-        <v>0.82162150062746497</v>
+        <v>0.92124552422109895</v>
       </c>
       <c r="J10">
-        <v>0.62299783841261602</v>
+        <v>0.69853815874917402</v>
       </c>
       <c r="K10">
-        <v>0.17859594656161801</v>
+        <v>0.14420450486491199</v>
       </c>
       <c r="L10">
-        <v>9.4425250650362696E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.5203938259717297E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2012</v>
       </c>
       <c r="B11">
-        <v>-0.46798639324517599</v>
+        <v>-0.50038096478319005</v>
       </c>
       <c r="C11">
-        <v>-0.48842400955642101</v>
+        <v>-0.52329670218551405</v>
       </c>
       <c r="D11">
-        <v>-0.47820520140079897</v>
+        <v>-0.511838833484352</v>
       </c>
       <c r="E11">
-        <v>4.6149299677630103E-2</v>
+        <v>7.6095193138347506E-2</v>
       </c>
       <c r="F11">
-        <v>-2.2614976634408101E-2</v>
+        <v>-1.00695393349661E-3</v>
       </c>
       <c r="G11">
-        <v>0.164694061268023</v>
+        <v>0.20901385574832701</v>
       </c>
       <c r="H11">
-        <v>-3.7011547059510798E-2</v>
+        <v>-1.7149150867402499E-2</v>
       </c>
       <c r="I11">
-        <v>0.45559022476639099</v>
+        <v>0.51083187955085496</v>
       </c>
       <c r="J11">
-        <v>0.44119365434128799</v>
+        <v>0.49468968261695001</v>
       </c>
       <c r="K11">
-        <v>6.8764276312038103E-2</v>
+        <v>7.7102147071844096E-2</v>
       </c>
       <c r="L11">
-        <v>0.20170560832753401</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.22616300661572999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2015</v>
       </c>
       <c r="B12">
-        <v>-0.32665449394178703</v>
+        <v>-0.34191215698850502</v>
       </c>
       <c r="C12">
-        <v>-0.30392219180543201</v>
+        <v>-0.31642349635539602</v>
       </c>
       <c r="D12">
-        <v>-0.31528834287361002</v>
+        <v>-0.32916782667195099</v>
       </c>
       <c r="E12">
-        <v>-2.5288425407807399E-2</v>
+        <v>-4.0045662341092001E-3</v>
       </c>
       <c r="F12">
-        <v>6.4092907057936299E-2</v>
+        <v>9.6214515691206301E-2</v>
       </c>
       <c r="G12">
-        <v>1.2451643438613399E-2</v>
+        <v>3.8311596965137099E-2</v>
       </c>
       <c r="H12">
-        <v>1.8321540770214501E-2</v>
+        <v>4.4893236613375499E-2</v>
       </c>
       <c r="I12">
-        <v>0.37938124993154598</v>
+        <v>0.42538234236315697</v>
       </c>
       <c r="J12">
-        <v>0.33360988364382399</v>
+        <v>0.37406106328532601</v>
       </c>
       <c r="K12">
-        <v>-8.9381332465743701E-2</v>
+        <v>-0.10021908192531501</v>
       </c>
       <c r="L12">
-        <v>-5.8698973316010901E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>-6.5816396482383296E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2016</v>
       </c>
       <c r="B13">
-        <v>-0.40741329002508397</v>
+        <v>-0.432463194633459</v>
       </c>
       <c r="C13">
-        <v>-0.46113141242808797</v>
+        <v>-0.49269479737941402</v>
       </c>
       <c r="D13">
-        <v>-0.43427235122658597</v>
+        <v>-0.46257899600643598</v>
       </c>
       <c r="E13">
-        <v>-0.53327753615491502</v>
+        <v>-0.57358885081214805</v>
       </c>
       <c r="F13">
-        <v>-0.568118145804692</v>
+        <v>-0.612653986858952</v>
       </c>
       <c r="G13">
-        <v>-0.55201439813785502</v>
+        <v>-0.59459761242141695</v>
       </c>
       <c r="H13">
-        <v>-0.53793657606869705</v>
+        <v>-0.578812813019151</v>
       </c>
       <c r="I13">
-        <v>-0.133845794578106</v>
+        <v>-0.15007499085251499</v>
       </c>
       <c r="J13">
-        <v>-0.10366422484211101</v>
+        <v>-0.116233817012715</v>
       </c>
       <c r="K13">
-        <v>3.4840609649776498E-2</v>
+        <v>3.9065136046803797E-2</v>
       </c>
       <c r="L13">
-        <v>-1.40778220691581E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>-1.57847994022654E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2017</v>
       </c>
       <c r="B14">
-        <v>-0.41033528479100401</v>
+        <v>-0.435739489859236</v>
       </c>
       <c r="C14">
-        <v>-0.42015287125788098</v>
+        <v>-0.44674748756177601</v>
       </c>
       <c r="D14">
-        <v>-0.41524407802444302</v>
+        <v>-0.441243488710506</v>
       </c>
       <c r="E14">
-        <v>6.7338560434223205E-2</v>
+        <v>9.9853714085836806E-2</v>
       </c>
       <c r="F14">
-        <v>0.109659255938342</v>
+        <v>9.5243897695961893E-2</v>
       </c>
       <c r="G14">
-        <v>3.6587022423846399E-2</v>
+        <v>6.5373461641932307E-2</v>
       </c>
       <c r="H14">
-        <v>-3.4993056089053801E-2</v>
+        <v>-1.48859119297724E-2</v>
       </c>
       <c r="I14">
-        <v>0.52490333396278499</v>
+        <v>0.53648738640646798</v>
       </c>
       <c r="J14">
-        <v>0.38025102193538901</v>
+        <v>0.42635757678073299</v>
       </c>
       <c r="K14">
-        <v>-4.2320695504118801E-2</v>
+        <v>4.6098163898748599E-3</v>
       </c>
       <c r="L14">
-        <v>7.15800785129002E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>8.0259373571704706E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2019</v>
       </c>
       <c r="B15">
-        <v>-0.41240689446772</v>
+        <v>-0.43806228830249699</v>
       </c>
       <c r="C15">
-        <v>-0.43087766337360001</v>
+        <v>-0.45877269226645101</v>
       </c>
       <c r="D15">
-        <v>-0.42164227892065997</v>
+        <v>-0.44841749028447397</v>
       </c>
       <c r="E15">
-        <v>-5.4685737683855601E-3</v>
+        <v>1.8218500712896699E-2</v>
       </c>
       <c r="F15">
-        <v>-9.0932179558833801E-2</v>
+        <v>-7.7607818654499394E-2</v>
       </c>
       <c r="G15">
-        <v>0.18893315417637199</v>
+        <v>0.23619200996647099</v>
       </c>
       <c r="H15">
-        <v>-0.135929021458293</v>
+        <v>-0.128060659983876</v>
       </c>
       <c r="I15">
-        <v>0.33071009936182599</v>
+        <v>0.37080967162997502</v>
       </c>
       <c r="J15">
-        <v>0.28571325746236698</v>
+        <v>0.32035683030059797</v>
       </c>
       <c r="K15">
-        <v>8.5463605790448205E-2</v>
+        <v>9.5826319367396204E-2</v>
       </c>
       <c r="L15">
-        <v>0.32486217563466602</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.364252669950346</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2020</v>
       </c>
       <c r="B16">
-        <v>-0.26952924339710399</v>
+        <v>-0.277860301792276</v>
       </c>
       <c r="C16">
-        <v>-0.28422179496905797</v>
+        <v>-0.29433436845766098</v>
       </c>
       <c r="D16">
-        <v>-0.27687551918308101</v>
+        <v>-0.28609733512496799</v>
       </c>
       <c r="E16">
-        <v>-0.41232664048582002</v>
+        <v>-0.43797230328924103</v>
       </c>
       <c r="F16">
-        <v>-0.33468163196573603</v>
+        <v>-0.35091260910814898</v>
       </c>
       <c r="G16">
-        <v>-0.304765230242871</v>
+        <v>-0.31736875568301098</v>
       </c>
       <c r="H16">
-        <v>-0.29021078623519297</v>
+        <v>-0.30104954253028798</v>
       </c>
       <c r="I16">
-        <v>-5.7806112782655003E-2</v>
+        <v>-6.4815273983180405E-2</v>
       </c>
       <c r="J16">
-        <v>-1.33352670521126E-2</v>
+        <v>-1.4952207405319501E-2</v>
       </c>
       <c r="K16">
-        <v>-7.7645008520084699E-2</v>
+        <v>-8.7059694181092204E-2</v>
       </c>
       <c r="L16">
-        <v>-1.45544440076779E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>-1.6319213152723201E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
+        <v>2021</v>
+      </c>
+      <c r="B17">
+        <v>-0.22161221556921301</v>
+      </c>
+      <c r="C17">
+        <v>-2.5968491742902802E-2</v>
+      </c>
+      <c r="D17">
+        <v>-0.12379035365605801</v>
+      </c>
+      <c r="E17">
+        <v>0.55481652365133305</v>
+      </c>
+      <c r="F17">
+        <v>0.58384319686473096</v>
+      </c>
+      <c r="G17">
+        <v>0.50776254221660799</v>
+      </c>
+      <c r="H17">
+        <v>0.28371979176486201</v>
+      </c>
+      <c r="I17">
+        <v>0.70763355052078902</v>
+      </c>
+      <c r="J17">
+        <v>0.40751014542092001</v>
+      </c>
+      <c r="K17">
+        <v>-2.9026673213397899E-2</v>
+      </c>
+      <c r="L17">
+        <v>0.22404275045174599</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2022</v>
+      </c>
+      <c r="B18">
+        <v>-0.44232397475888302</v>
+      </c>
+      <c r="C18">
+        <v>-0.473265720831615</v>
+      </c>
+      <c r="D18">
+        <v>-0.45779484779524898</v>
+      </c>
+      <c r="E18">
+        <v>0.216395761632763</v>
+      </c>
+      <c r="F18">
+        <v>0.284912644022568</v>
+      </c>
+      <c r="G18">
+        <v>0.40722016623094098</v>
+      </c>
+      <c r="H18">
+        <v>0.313567744549198</v>
+      </c>
+      <c r="I18">
+        <v>0.74270749181781703</v>
+      </c>
+      <c r="J18">
+        <v>0.77136259234444704</v>
+      </c>
+      <c r="K18">
+        <v>-6.8516882389804801E-2</v>
+      </c>
+      <c r="L18">
+        <v>9.3652421681743495E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>2023</v>
       </c>
-      <c r="B17">
-        <v>-0.47014772948760197</v>
-      </c>
-      <c r="C17">
-        <v>-0.44436358761848199</v>
-      </c>
-      <c r="D17">
-        <v>-0.45725565855304201</v>
-      </c>
-      <c r="E17">
-        <v>-1.7274136690394199E-2</v>
-      </c>
-      <c r="F17">
-        <v>4.8251193332018598E-2</v>
-      </c>
-      <c r="G17">
-        <v>-5.0648335795242097E-2</v>
-      </c>
-      <c r="H17">
-        <v>-0.103616779731876</v>
-      </c>
-      <c r="I17">
-        <v>0.50550685188506095</v>
-      </c>
-      <c r="J17">
-        <v>0.35363887882116701</v>
-      </c>
-      <c r="K17">
-        <v>-6.55253300224128E-2</v>
-      </c>
-      <c r="L17">
-        <v>5.2968443936633497E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B19">
+        <v>-0.502804369402167</v>
+      </c>
+      <c r="C19">
+        <v>-0.473893824492293</v>
+      </c>
+      <c r="D19">
+        <v>-0.48834909694723</v>
+      </c>
+      <c r="E19">
+        <v>-3.24394403473479E-2</v>
+      </c>
+      <c r="F19">
+        <v>-9.1830463907848797E-2</v>
+      </c>
+      <c r="G19">
+        <v>4.9814785627884601E-3</v>
+      </c>
+      <c r="H19">
+        <v>7.8451947580648801E-2</v>
+      </c>
+      <c r="I19">
+        <v>0.39651863303938101</v>
+      </c>
+      <c r="J19">
+        <v>0.56680104452787905</v>
+      </c>
+      <c r="K19">
+        <v>5.9391023560500897E-2</v>
+      </c>
+      <c r="L19">
+        <v>-7.3470469017860404E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2024</v>
+      </c>
+      <c r="B20">
+        <v>-0.39814428333115898</v>
+      </c>
+      <c r="C20">
+        <v>-0.35876933176318299</v>
+      </c>
+      <c r="D20">
+        <v>-0.37845680754717098</v>
+      </c>
+      <c r="E20">
+        <v>0.93581715438539403</v>
+      </c>
+      <c r="F20">
+        <v>0.30941907287502701</v>
+      </c>
+      <c r="G20">
+        <v>0.72428303915655001</v>
+      </c>
+      <c r="H20">
+        <v>0.35567575994742301</v>
+      </c>
+      <c r="I20">
+        <v>0.68787588042219805</v>
+      </c>
+      <c r="J20">
+        <v>0.73413256749459399</v>
+      </c>
+      <c r="K20">
+        <v>0.62639808151036702</v>
+      </c>
+      <c r="L20">
+        <v>0.368607279209127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2025</v>
+      </c>
+      <c r="B21">
+        <v>-0.40453022277353101</v>
+      </c>
+      <c r="C21">
+        <v>-0.52200804309101001</v>
+      </c>
+      <c r="D21">
+        <v>-0.46326913293227001</v>
+      </c>
+      <c r="E21">
+        <v>0.45753832347562401</v>
+      </c>
+      <c r="F21">
+        <v>0.62174106404952001</v>
+      </c>
+      <c r="G21">
+        <v>0.29374521118677699</v>
+      </c>
+      <c r="H21">
+        <v>0.440041866341014</v>
+      </c>
+      <c r="I21">
+        <v>1.08501019698179</v>
+      </c>
+      <c r="J21">
+        <v>0.90331099927328395</v>
+      </c>
+      <c r="K21">
+        <v>-0.164202740573896</v>
+      </c>
+      <c r="L21">
+        <v>-0.14629665515423701</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2026</v>
+      </c>
+      <c r="B22">
+        <v>-0.49935791463567197</v>
+      </c>
+      <c r="C22">
+        <v>-0.269617922622439</v>
+      </c>
+      <c r="D22">
+        <v>-0.38448791862905501</v>
+      </c>
+      <c r="E22">
+        <v>0.23751356555939401</v>
+      </c>
+      <c r="F22">
+        <v>-4.0344053904957699E-3</v>
+      </c>
+      <c r="G22">
+        <v>0.37972561298290602</v>
+      </c>
+      <c r="H22">
+        <v>-0.139561585224759</v>
+      </c>
+      <c r="I22">
+        <v>0.38045351323856003</v>
+      </c>
+      <c r="J22">
+        <v>0.24492633340429601</v>
+      </c>
+      <c r="K22">
+        <v>0.24154797094989</v>
+      </c>
+      <c r="L22">
+        <v>0.519287198207665</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2027</v>
+      </c>
+      <c r="B23">
+        <v>-0.20104567075202601</v>
+      </c>
+      <c r="C23">
+        <v>2.9813144337421601E-2</v>
+      </c>
+      <c r="D23">
+        <v>-8.5616263207302298E-2</v>
+      </c>
+      <c r="E23">
+        <v>1.0602487318374301</v>
+      </c>
+      <c r="F23">
+        <v>1.04706145230488</v>
+      </c>
+      <c r="G23">
+        <v>0.78818525028946096</v>
+      </c>
+      <c r="H23">
+        <v>0.63620901737457103</v>
+      </c>
+      <c r="I23">
+        <v>1.1326777155121801</v>
+      </c>
+      <c r="J23">
+        <v>0.72182528058187401</v>
+      </c>
+      <c r="K23">
+        <v>1.3187279532548101E-2</v>
+      </c>
+      <c r="L23">
+        <v>0.15197623291488899</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2028</v>
+      </c>
+      <c r="B24">
+        <v>-0.37802756103208701</v>
+      </c>
+      <c r="C24">
+        <v>-0.44465163835463001</v>
+      </c>
+      <c r="D24">
+        <v>-0.41133959969335898</v>
+      </c>
+      <c r="E24">
+        <v>0.34373101591038702</v>
+      </c>
+      <c r="F24">
+        <v>0.19076729886688901</v>
+      </c>
+      <c r="G24">
+        <v>0.17907855096888101</v>
+      </c>
+      <c r="H24">
+        <v>0.14520978228531101</v>
+      </c>
+      <c r="I24">
+        <v>0.60210689856024802</v>
+      </c>
+      <c r="J24">
+        <v>0.55654938197866999</v>
+      </c>
+      <c r="K24">
+        <v>0.15296371704349801</v>
+      </c>
+      <c r="L24">
+        <v>3.3868768683570097E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2029</v>
+      </c>
+      <c r="B25">
+        <v>-0.44130328535136099</v>
+      </c>
+      <c r="C25">
+        <v>-0.31086954629750402</v>
+      </c>
+      <c r="D25">
+        <v>-0.37608641582443197</v>
+      </c>
+      <c r="E25">
+        <v>0.513841099393475</v>
+      </c>
+      <c r="F25">
+        <v>0.42262664961353602</v>
+      </c>
+      <c r="G25">
+        <v>0.20552284894907999</v>
+      </c>
+      <c r="H25">
+        <v>5.4352592166751E-2</v>
+      </c>
+      <c r="I25">
+        <v>0.79871306543796805</v>
+      </c>
+      <c r="J25">
+        <v>0.43043900799118301</v>
+      </c>
+      <c r="K25">
+        <v>9.1214449779939102E-2</v>
+      </c>
+      <c r="L25">
+        <v>0.15117025678232901</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2031</v>
+      </c>
+      <c r="B26">
+        <v>-0.45141245384501599</v>
+      </c>
+      <c r="C26">
+        <v>-0.46992373531631099</v>
+      </c>
+      <c r="D26">
+        <v>-0.46066809458066299</v>
+      </c>
+      <c r="E26">
+        <v>0.215187245658542</v>
+      </c>
+      <c r="F26">
+        <v>5.7538362267163599E-2</v>
+      </c>
+      <c r="G26">
+        <v>0.14484549305960001</v>
+      </c>
+      <c r="H26">
+        <v>-1.7711371358659401E-2</v>
+      </c>
+      <c r="I26">
+        <v>0.51820645684782696</v>
+      </c>
+      <c r="J26">
+        <v>0.44295672322200402</v>
+      </c>
+      <c r="K26">
+        <v>0.157648883391378</v>
+      </c>
+      <c r="L26">
+        <v>0.16255686441826001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B19">
-        <f t="shared" ref="B19:L19" si="0">AVERAGE(B2:B17)</f>
-        <v>-0.29552613970811242</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>-0.21567109841496696</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>-0.25559861906153986</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>0.15590611689748518</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>9.233215831901824E-2</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="0"/>
-        <v>6.1251864965107802E-2</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="0"/>
-        <v>-3.0950984034277273E-2</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="0"/>
-        <v>0.34793077738055794</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="0"/>
-        <v>0.22464763502726237</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="0"/>
-        <v>6.3573958578466774E-2</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="0"/>
-        <v>9.2202848999385148E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="B29">
+        <f>AVERAGE(B2:B26)</f>
+        <v>-0.33651823554070581</v>
+      </c>
+      <c r="C29">
+        <f>AVERAGE(C2:C26)</f>
+        <v>-0.26086239761785246</v>
+      </c>
+      <c r="D29">
+        <f>AVERAGE(D2:D26)</f>
+        <v>-0.29869031657927914</v>
+      </c>
+      <c r="E29">
+        <f>AVERAGE(E2:E26)</f>
+        <v>0.2829173512880499</v>
+      </c>
+      <c r="F29">
+        <f>AVERAGE(F2:F26)</f>
+        <v>0.21350306603728267</v>
+      </c>
+      <c r="G29">
+        <f>AVERAGE(G2:G26)</f>
+        <v>0.20422331217587841</v>
+      </c>
+      <c r="H29">
+        <f>AVERAGE(H2:H26)</f>
+        <v>8.304505525377022E-2</v>
+      </c>
+      <c r="I29">
+        <f>AVERAGE(I2:I26)</f>
+        <v>0.51219338261656189</v>
+      </c>
+      <c r="J29">
+        <f>AVERAGE(J2:J26)</f>
+        <v>0.38173537183304929</v>
+      </c>
+      <c r="K29">
+        <f>AVERAGE(K2:K26)</f>
+        <v>6.9414285250767108E-2</v>
+      </c>
+      <c r="L29">
+        <f>AVERAGE(L2:L26)</f>
+        <v>0.12117825692210821</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B20">
-        <f t="shared" ref="B20:L20" si="1">STDEV(B2:B17)</f>
-        <v>0.25356999981064537</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="1"/>
-        <v>0.38031445024191934</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="1"/>
-        <v>0.27606849012853285</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="1"/>
-        <v>0.56564419504352237</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="1"/>
-        <v>0.41944900523581752</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="1"/>
-        <v>0.39593838845519053</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="1"/>
-        <v>0.3187086938114691</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="1"/>
-        <v>0.41044698779122535</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="1"/>
-        <v>0.32837874643636078</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="1"/>
-        <v>0.18937728181390884</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="1"/>
-        <v>0.13416360878192829</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B30">
+        <f>STDEV(B2:B26)</f>
+        <v>0.22432785364610394</v>
+      </c>
+      <c r="C30">
+        <f>STDEV(C2:C26)</f>
+        <v>0.3425110515703807</v>
+      </c>
+      <c r="D30">
+        <f>STDEV(D2:D26)</f>
+        <v>0.24925725433009538</v>
+      </c>
+      <c r="E30">
+        <f>STDEV(E2:E26)</f>
+        <v>0.51629246015634467</v>
+      </c>
+      <c r="F30">
+        <f>STDEV(F2:F26)</f>
+        <v>0.44010302026369058</v>
+      </c>
+      <c r="G30">
+        <f>STDEV(G2:G26)</f>
+        <v>0.40256167783215246</v>
+      </c>
+      <c r="H30">
+        <f>STDEV(H2:H26)</f>
+        <v>0.33479471653856119</v>
+      </c>
+      <c r="I30">
+        <f>STDEV(I2:I26)</f>
+        <v>0.42064111733403731</v>
+      </c>
+      <c r="J30">
+        <f>STDEV(J2:J26)</f>
+        <v>0.34886701802774905</v>
+      </c>
+      <c r="K30">
+        <f>STDEV(K2:K26)</f>
+        <v>0.17853340417476013</v>
+      </c>
+      <c r="L30">
+        <f>STDEV(L2:L26)</f>
+        <v>0.17035211380920443</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B21">
-        <f t="shared" ref="B21:L21" si="2">B20/(SQRT(16))</f>
-        <v>6.3392499952661344E-2</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="2"/>
-        <v>9.5078612560479836E-2</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="2"/>
-        <v>6.9017122532133213E-2</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="2"/>
-        <v>0.14141104876088059</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="2"/>
-        <v>0.10486225130895438</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="2"/>
-        <v>9.8984597113797632E-2</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="2"/>
-        <v>7.9677173452867275E-2</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="2"/>
-        <v>0.10261174694780634</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="2"/>
-        <v>8.2094686609090195E-2</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="2"/>
-        <v>4.7344320453477209E-2</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="2"/>
-        <v>3.3540902195482072E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="B31">
+        <f>B30/SQRT(25)</f>
+        <v>4.4865570729220788E-2</v>
+      </c>
+      <c r="C31">
+        <f>C30/SQRT(25)</f>
+        <v>6.8502210314076134E-2</v>
+      </c>
+      <c r="D31">
+        <f>D30/SQRT(25)</f>
+        <v>4.9851450866019074E-2</v>
+      </c>
+      <c r="E31">
+        <f>E30/SQRT(25)</f>
+        <v>0.10325849203126894</v>
+      </c>
+      <c r="F31">
+        <f>F30/SQRT(25)</f>
+        <v>8.8020604052738122E-2</v>
+      </c>
+      <c r="G31">
+        <f>G30/SQRT(25)</f>
+        <v>8.051233556643049E-2</v>
+      </c>
+      <c r="H31">
+        <f>H30/SQRT(25)</f>
+        <v>6.6958943307712238E-2</v>
+      </c>
+      <c r="I31">
+        <f>I30/SQRT(25)</f>
+        <v>8.4128223466807456E-2</v>
+      </c>
+      <c r="J31">
+        <f>J30/SQRT(25)</f>
+        <v>6.9773403605549816E-2</v>
+      </c>
+      <c r="K31">
+        <f>K30/SQRT(25)</f>
+        <v>3.5706680834952029E-2</v>
+      </c>
+      <c r="L31">
+        <f>L30/SQRT(25)</f>
+        <v>3.4070422761840885E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B22">
-        <f t="shared" ref="B22:L22" si="3">B21*1.96</f>
-        <v>0.12424929990721623</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="3"/>
-        <v>0.18635408061854047</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="3"/>
-        <v>0.13527356016298109</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="3"/>
-        <v>0.27716565557132594</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="3"/>
-        <v>0.20553001256555059</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="3"/>
-        <v>0.19400981034304335</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="3"/>
-        <v>0.15616725996761985</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="3"/>
-        <v>0.2011190240177004</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="3"/>
-        <v>0.16090558575381678</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="3"/>
-        <v>9.2794868088815333E-2</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="3"/>
-        <v>6.5740168303144858E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B32">
+        <f>B31*1.96</f>
+        <v>8.793651862927275E-2</v>
+      </c>
+      <c r="C32">
+        <f>C31*1.96</f>
+        <v>0.13426433221558923</v>
+      </c>
+      <c r="D32">
+        <f>D31*1.96</f>
+        <v>9.770884369739738E-2</v>
+      </c>
+      <c r="E32">
+        <f>E31*1.96</f>
+        <v>0.20238664438128712</v>
+      </c>
+      <c r="F32">
+        <f>F31*1.96</f>
+        <v>0.17252038394336672</v>
+      </c>
+      <c r="G32">
+        <f>G31*1.96</f>
+        <v>0.15780417771020375</v>
+      </c>
+      <c r="H32">
+        <f>H31*1.96</f>
+        <v>0.13123952888311599</v>
+      </c>
+      <c r="I32">
+        <f>I31*1.96</f>
+        <v>0.16489131799494261</v>
+      </c>
+      <c r="J32">
+        <f>J31*1.96</f>
+        <v>0.13675587106687764</v>
+      </c>
+      <c r="K32">
+        <f>K31*1.96</f>
+        <v>6.9985094436505982E-2</v>
+      </c>
+      <c r="L32">
+        <f>L31*1.96</f>
+        <v>6.677802861320814E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B23">
-        <v>-0.1712768398008962</v>
-      </c>
-      <c r="C23">
-        <v>-2.9317017796426481E-2</v>
-      </c>
-      <c r="D23">
-        <v>-0.12032505889855877</v>
-      </c>
-      <c r="E23">
-        <v>0.43307177246881112</v>
-      </c>
-      <c r="F23">
-        <v>0.29786217088456884</v>
-      </c>
-      <c r="G23">
-        <v>0.25526167530815114</v>
-      </c>
-      <c r="H23">
-        <v>0.12521627593334259</v>
-      </c>
-      <c r="I23">
-        <v>0.54904980139825832</v>
-      </c>
-      <c r="J23">
-        <v>0.38555322078107912</v>
-      </c>
-      <c r="K23">
-        <v>0.15636882666728211</v>
-      </c>
-      <c r="L23">
-        <v>0.15794301730253002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B33">
+        <f>B29+B32</f>
+        <v>-0.24858171691143305</v>
+      </c>
+      <c r="C33">
+        <f>C29+C32</f>
+        <v>-0.12659806540226323</v>
+      </c>
+      <c r="D33">
+        <f>D29+D32</f>
+        <v>-0.20098147288188176</v>
+      </c>
+      <c r="E33">
+        <f>E29+E32</f>
+        <v>0.48530399566933702</v>
+      </c>
+      <c r="F33">
+        <f>F29+F32</f>
+        <v>0.38602344998064941</v>
+      </c>
+      <c r="G33">
+        <f>G29+G32</f>
+        <v>0.36202748988608213</v>
+      </c>
+      <c r="H33">
+        <f>H29+H32</f>
+        <v>0.21428458413688622</v>
+      </c>
+      <c r="I33">
+        <f>I29+I32</f>
+        <v>0.6770847006115045</v>
+      </c>
+      <c r="J33">
+        <f>J29+J32</f>
+        <v>0.51849124289992687</v>
+      </c>
+      <c r="K33">
+        <f>K29+K32</f>
+        <v>0.13939937968727309</v>
+      </c>
+      <c r="L33">
+        <f>L29+L32</f>
+        <v>0.18795628553531635</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B24">
-        <v>-0.41977543961532865</v>
-      </c>
-      <c r="C24">
-        <v>-0.40202517903350743</v>
-      </c>
-      <c r="D24">
-        <v>-0.39087217922452094</v>
-      </c>
-      <c r="E24">
-        <v>-0.12125953867384076</v>
-      </c>
-      <c r="F24">
-        <v>-0.11319785424653235</v>
-      </c>
-      <c r="G24">
-        <v>-0.13275794537793556</v>
-      </c>
-      <c r="H24">
-        <v>-0.18711824400189711</v>
-      </c>
-      <c r="I24">
-        <v>0.14681175336285754</v>
-      </c>
-      <c r="J24">
-        <v>6.3742049273445595E-2</v>
-      </c>
-      <c r="K24">
-        <v>-2.9220909510348558E-2</v>
-      </c>
-      <c r="L24">
-        <v>2.646268069624029E-2</v>
+      <c r="B34">
+        <f>B29-B32</f>
+        <v>-0.42445475416997858</v>
+      </c>
+      <c r="C34">
+        <f>C29-C32</f>
+        <v>-0.39512672983344166</v>
+      </c>
+      <c r="D34">
+        <f>D29-D32</f>
+        <v>-0.39639916027667654</v>
+      </c>
+      <c r="E34">
+        <f>E29-E32</f>
+        <v>8.0530706906762783E-2</v>
+      </c>
+      <c r="F34">
+        <f>F29-F32</f>
+        <v>4.0982682093915951E-2</v>
+      </c>
+      <c r="G34">
+        <f>G29-G32</f>
+        <v>4.6419134465674666E-2</v>
+      </c>
+      <c r="H34">
+        <f>H29-H32</f>
+        <v>-4.8194473629345772E-2</v>
+      </c>
+      <c r="I34">
+        <f>I29-I32</f>
+        <v>0.34730206462161928</v>
+      </c>
+      <c r="J34">
+        <f>J29-J32</f>
+        <v>0.24497950076617164</v>
+      </c>
+      <c r="K34">
+        <f>K29-K32</f>
+        <v>-5.7080918573887418E-4</v>
+      </c>
+      <c r="L34">
+        <f>L29-L32</f>
+        <v>5.4400228308900067E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>